<commit_message>
Completed the Enhancing and written the Automation script for the Exam Submission at Exam Taker side
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/User_Details.xlsx
+++ b/src/test/resources/ExcelFiles/User_Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://focalpointk12-my.sharepoint.com/personal/sahoo_suryakanta_focalpointk12_com/Documents/FP_Automation_Script/ExamCenter_Automation/src/test/resources/ExcelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{607780A2-CDA5-42DE-9DE1-D20D6D1EC8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF17E72A-91BA-4D51-989C-6799D1A1CCB0}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{607780A2-CDA5-42DE-9DE1-D20D6D1EC8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF56BD8E-AE58-4C32-92A9-E48395CAE9A2}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="2688" windowWidth="20532" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="20532" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STAGE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>FirstName</t>
   </si>
@@ -43,18 +43,9 @@
     <t>TestName</t>
   </si>
   <si>
-    <t>Grade</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
     <t>User Role</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>stage</t>
   </si>
   <si>
@@ -64,9 +55,6 @@
     <t>@Abcd1234</t>
   </si>
   <si>
-    <t>S.No.</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -79,51 +67,44 @@
     <t>fpkcontroller</t>
   </si>
   <si>
-    <t>79606</t>
-  </si>
-  <si>
     <t>FPKproctor</t>
   </si>
   <si>
-    <t>819520</t>
-  </si>
-  <si>
     <t>ExamTaker</t>
   </si>
   <si>
-    <t>552256</t>
-  </si>
-  <si>
-    <t>794036</t>
-  </si>
-  <si>
     <t>FPKexamtaker</t>
   </si>
   <si>
-    <t>339751</t>
-  </si>
-  <si>
-    <t>975719</t>
-  </si>
-  <si>
-    <t>355626</t>
-  </si>
-  <si>
-    <t>848820</t>
-  </si>
-  <si>
-    <t>974900</t>
-  </si>
-  <si>
-    <t>892259</t>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>430836</t>
+  </si>
+  <si>
+    <t>88412</t>
+  </si>
+  <si>
+    <t>602415</t>
+  </si>
+  <si>
+    <t>ExamName</t>
+  </si>
+  <si>
+    <t>ScheduleName</t>
+  </si>
+  <si>
+    <t>FPK12Exam80339</t>
+  </si>
+  <si>
+    <t>FPK12Schedule15128</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,19 +113,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,12 +139,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -181,26 +173,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -217,6 +236,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,99 +505,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H2" sqref="H2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0"/>
-    <col min="2" max="2" customWidth="true" width="42.5546875"/>
-    <col min="3" max="3" customWidth="true" width="19.5546875"/>
-    <col min="4" max="4" customWidth="true" width="14.44140625"/>
-    <col min="5" max="5" customWidth="true" width="16.44140625"/>
-    <col min="7" max="7" customWidth="true" width="12.44140625"/>
+    <col min="1" max="1" width="42.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="35.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
+      <c r="G4" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" t="s" s="0">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0">
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C5" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>23</v>
+      <c r="G5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>